<commit_message>
Update with China news
</commit_message>
<xml_diff>
--- a/€AIR.xlsx
+++ b/€AIR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54120EDF-4B85-48A3-B280-573103F70463}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D80F32E-301B-4075-BC24-6149F565A7E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{7A999692-C6C4-4F97-8931-23E590A5D765}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{7A999692-C6C4-4F97-8931-23E590A5D765}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="89">
   <si>
     <t>€AIR</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Balance Sheet</t>
+  </si>
+  <si>
+    <t>Airbus starts A321 production in Tianjin, China</t>
   </si>
 </sst>
 </file>
@@ -499,7 +502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -543,33 +546,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -604,6 +580,37 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1092,8 +1099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E59CE47-24E0-472A-A3E5-76E7FAE52578}">
   <dimension ref="B2:W36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1113,32 +1120,32 @@
       </c>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="G4" s="31" t="s">
+      <c r="G4" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="33"/>
-      <c r="T4" s="31" t="s">
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="47"/>
+      <c r="T4" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="33"/>
+      <c r="U4" s="46"/>
+      <c r="V4" s="46"/>
+      <c r="W4" s="47"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="32"/>
-      <c r="D5" s="33"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
       <c r="G5" s="17"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -1165,8 +1172,12 @@
         <v>100.92</v>
       </c>
       <c r="D6" s="7"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="12"/>
+      <c r="G6" s="54">
+        <v>44866</v>
+      </c>
+      <c r="H6" s="55" t="s">
+        <v>88</v>
+      </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -1361,11 +1372,11 @@
       <c r="W14" s="13"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
       <c r="G15" s="17"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -1386,10 +1397,10 @@
       <c r="B16" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="30"/>
+      <c r="D16" s="49"/>
       <c r="G16" s="17"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -1412,10 +1423,10 @@
       <c r="B17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="30"/>
+      <c r="D17" s="49"/>
       <c r="G17" s="17"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -1436,10 +1447,10 @@
       <c r="B18" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D18" s="30"/>
+      <c r="D18" s="49"/>
       <c r="G18" s="17"/>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -1460,10 +1471,10 @@
       <c r="B19" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="30"/>
+      <c r="D19" s="49"/>
       <c r="G19" s="17"/>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -1484,10 +1495,10 @@
       <c r="B20" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="26"/>
+      <c r="D20" s="51"/>
       <c r="G20" s="17"/>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -1539,11 +1550,11 @@
       <c r="W22" s="13"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="32"/>
-      <c r="D23" s="33"/>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
       <c r="G23" s="17"/>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -1564,10 +1575,10 @@
       <c r="B24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="29" t="s">
+      <c r="C24" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="30"/>
+      <c r="D24" s="49"/>
       <c r="G24" s="17"/>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -1588,10 +1599,10 @@
       <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="29">
+      <c r="C25" s="48">
         <v>1970</v>
       </c>
-      <c r="D25" s="30"/>
+      <c r="D25" s="49"/>
       <c r="G25" s="17"/>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -1694,10 +1705,10 @@
       <c r="B30" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="53"/>
       <c r="G30" s="17"/>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -1749,11 +1760,11 @@
       <c r="W32" s="13"/>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="32"/>
-      <c r="D33" s="33"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
       <c r="G33" s="17"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -1855,10 +1866,11 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C30:D30" r:id="rId1" display="Link" xr:uid="{D9D5318B-D4EA-4E8E-B757-32C8AE640F18}"/>
+    <hyperlink ref="H6" r:id="rId2" location="Echobox=1668050112" xr:uid="{69C938F5-4E55-4EBE-BED7-07B738A18FA5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1866,11 +1878,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2073C80-13D3-405E-87ED-FCD88E0B1020}">
   <dimension ref="A1:AF154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1880,177 +1892,177 @@
     <col min="3" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="34" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="47" t="s">
+    <row r="1" spans="1:32" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="I1" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="J1" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="L1" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="34" t="s">
+      <c r="M1" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="34" t="s">
+      <c r="R1" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="34" t="s">
+      <c r="S1" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="T1" s="34" t="s">
+      <c r="T1" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="U1" s="43" t="s">
+      <c r="U1" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="V1" s="34" t="s">
+      <c r="V1" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="W1" s="34" t="s">
+      <c r="W1" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="X1" s="34" t="s">
+      <c r="X1" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="Y1" s="34" t="s">
+      <c r="Y1" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="Z1" s="34" t="s">
+      <c r="Z1" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="AA1" s="34" t="s">
+      <c r="AA1" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AB1" s="34" t="s">
+      <c r="AB1" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="AC1" s="34" t="s">
+      <c r="AC1" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="AD1" s="34" t="s">
+      <c r="AD1" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="AE1" s="34" t="s">
+      <c r="AE1" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="AF1" s="34" t="s">
+      <c r="AF1" s="25" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="35" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="T2" s="45">
+    <row r="2" spans="1:32" s="26" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="T2" s="36">
         <v>44196</v>
       </c>
-      <c r="U2" s="45">
+      <c r="U2" s="36">
         <v>44561</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="35" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
-      <c r="U3" s="44">
+    <row r="3" spans="1:32" s="26" customFormat="1" ht="11.25" x14ac:dyDescent="0.2">
+      <c r="U3" s="35">
         <v>44609</v>
       </c>
     </row>
-    <row r="4" spans="1:32" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="48"/>
-      <c r="B4" s="49" t="s">
+    <row r="4" spans="1:32" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="39"/>
+      <c r="B4" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="50"/>
-      <c r="T4" s="49">
+      <c r="C4" s="41"/>
+      <c r="T4" s="40">
         <v>49912</v>
       </c>
-      <c r="U4" s="49">
+      <c r="U4" s="40">
         <v>52149</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A5" s="36"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="T5" s="52">
+      <c r="T5" s="43">
         <v>44250</v>
       </c>
-      <c r="U5" s="52">
+      <c r="U5" s="43">
         <v>42518</v>
       </c>
     </row>
     <row r="6" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="T6" s="49">
+      <c r="T6" s="40">
         <f t="shared" ref="T6" si="0">T4-T5</f>
         <v>5662</v>
       </c>
-      <c r="U6" s="49">
+      <c r="U6" s="40">
         <f>U4-U5</f>
         <v>9631</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A7" s="36"/>
+      <c r="A7" s="27"/>
       <c r="B7" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="T7" s="52">
+      <c r="T7" s="43">
         <v>717</v>
       </c>
-      <c r="U7" s="52">
+      <c r="U7" s="43">
         <v>713</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A8" s="36"/>
+      <c r="A8" s="27"/>
       <c r="B8" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="T8" s="52">
+      <c r="T8" s="43">
         <v>1423</v>
       </c>
-      <c r="U8" s="52">
+      <c r="U8" s="43">
         <v>1339</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A9" s="37"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="T9" s="52">
+      <c r="T9" s="43">
         <v>2858</v>
       </c>
-      <c r="U9" s="52">
+      <c r="U9" s="43">
         <v>2746</v>
       </c>
     </row>
@@ -2058,10 +2070,10 @@
       <c r="B10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="T10" s="52">
+      <c r="T10" s="43">
         <v>132</v>
       </c>
-      <c r="U10" s="52">
+      <c r="U10" s="43">
         <v>594</v>
       </c>
     </row>
@@ -2070,10 +2082,10 @@
       <c r="B11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="T11" s="52">
+      <c r="T11" s="43">
         <v>1458</v>
       </c>
-      <c r="U11" s="52">
+      <c r="U11" s="43">
         <v>201</v>
       </c>
     </row>
@@ -2081,11 +2093,11 @@
       <c r="B12" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="T12" s="49">
+      <c r="T12" s="40">
         <f>T6-T7-T8-T9+T10-T11</f>
         <v>-662</v>
       </c>
-      <c r="U12" s="49">
+      <c r="U12" s="40">
         <f>U6-U7-U8-U9+U10-U11</f>
         <v>5226</v>
       </c>
@@ -2119,7 +2131,7 @@
       <c r="T15" s="1">
         <v>140</v>
       </c>
-      <c r="U15" s="52">
+      <c r="U15" s="43">
         <v>88</v>
       </c>
     </row>
@@ -2149,11 +2161,11 @@
       <c r="B18" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="T18" s="52">
+      <c r="T18" s="43">
         <f>T15-T16-T17</f>
         <v>-620</v>
       </c>
-      <c r="U18" s="52">
+      <c r="U18" s="43">
         <f>U15-U16-U17</f>
         <v>-315</v>
       </c>
@@ -2162,11 +2174,11 @@
       <c r="B19" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="T19" s="52">
+      <c r="T19" s="43">
         <f>T12+T13+T14+T18</f>
         <v>-1130</v>
       </c>
-      <c r="U19" s="52">
+      <c r="U19" s="43">
         <f>U12+U13+U14+U18</f>
         <v>5027</v>
       </c>
@@ -2186,11 +2198,11 @@
       <c r="B21" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="T21" s="49">
+      <c r="T21" s="40">
         <f>T19-T20</f>
         <v>-1169</v>
       </c>
-      <c r="U21" s="49">
+      <c r="U21" s="40">
         <f>U19-U20</f>
         <v>4174</v>
       </c>
@@ -2209,7 +2221,7 @@
       <c r="B26" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="U26" s="51">
+      <c r="U26" s="42">
         <f>U4/T4-1</f>
         <v>4.4818881230966445E-2</v>
       </c>
@@ -2224,11 +2236,11 @@
       <c r="B29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="T29" s="38">
-        <f t="shared" ref="T29:U29" si="1">T6/T4</f>
+      <c r="T29" s="29">
+        <f t="shared" ref="T29" si="1">T6/T4</f>
         <v>0.11343965379067159</v>
       </c>
-      <c r="U29" s="38">
+      <c r="U29" s="29">
         <f>U6/U4</f>
         <v>0.18468235248998063</v>
       </c>
@@ -2237,11 +2249,11 @@
       <c r="B30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="T30" s="38">
-        <f t="shared" ref="T30:U30" si="2">T12/T4</f>
+      <c r="T30" s="29">
+        <f t="shared" ref="T30" si="2">T12/T4</f>
         <v>-1.3263343484532777E-2</v>
       </c>
-      <c r="U30" s="38">
+      <c r="U30" s="29">
         <f>U12/U4</f>
         <v>0.1002128516366565</v>
       </c>
@@ -2250,11 +2262,11 @@
       <c r="B31" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="T31" s="38">
-        <f t="shared" ref="T31:U31" si="3">T21/T4</f>
+      <c r="T31" s="29">
+        <f t="shared" ref="T31" si="3">T21/T4</f>
         <v>-2.3421221349575253E-2</v>
       </c>
-      <c r="U31" s="38">
+      <c r="U31" s="29">
         <f>U21/U4</f>
         <v>8.0039885712094194E-2</v>
       </c>
@@ -2263,11 +2275,11 @@
       <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="T32" s="38">
-        <f t="shared" ref="T32:U32" si="4">T20/T19</f>
+      <c r="T32" s="29">
+        <f t="shared" ref="T32" si="4">T20/T19</f>
         <v>-3.4513274336283185E-2</v>
       </c>
-      <c r="U32" s="38">
+      <c r="U32" s="29">
         <f>U20/U19</f>
         <v>0.16968370797692461</v>
       </c>
@@ -2279,7 +2291,7 @@
       <c r="A35" s="3"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B36" s="53" t="s">
+      <c r="B36" s="44" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2287,61 +2299,61 @@
       <c r="A41" s="3"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="38"/>
+      <c r="A42" s="29"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="39"/>
+      <c r="A43" s="30"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="38"/>
+      <c r="A44" s="29"/>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="3"/>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="40"/>
+      <c r="A55" s="31"/>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="41"/>
+      <c r="A56" s="32"/>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="41"/>
+      <c r="A57" s="32"/>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="41"/>
+      <c r="A58" s="32"/>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="41"/>
+      <c r="A59" s="32"/>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="41"/>
+      <c r="A60" s="32"/>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="41"/>
+      <c r="A61" s="32"/>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="41"/>
+      <c r="A62" s="32"/>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="40"/>
+      <c r="A63" s="31"/>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="41"/>
+      <c r="A64" s="32"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="41"/>
+      <c r="A65" s="32"/>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="41"/>
+      <c r="A66" s="32"/>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="41"/>
+      <c r="A67" s="32"/>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
+      <c r="A68" s="31"/>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="41"/>
+      <c r="A69" s="32"/>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" s="3"/>
@@ -2374,19 +2386,19 @@
       <c r="A118" s="3"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A135" s="41"/>
+      <c r="A135" s="32"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="41"/>
+      <c r="A136" s="32"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="3"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A145" s="42"/>
+      <c r="A145" s="33"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A146" s="42"/>
+      <c r="A146" s="33"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="3"/>

</xml_diff>